<commit_message>
feat: fix MVP Map & Add Monster Spawnner
</commit_message>
<xml_diff>
--- a/INFEST_Project/Util/ExcelToJsonWizard.v1.0.6/excel_files/ConsumeItem.xlsx
+++ b/INFEST_Project/Util/ExcelToJsonWizard.v1.0.6/excel_files/ConsumeItem.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr codeName="현재_통합_문서" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\worni\Desktop\포트폴리오\내배캠\새 폴더\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\worni\Desktop\GitProject\INFEST\INFEST_Project\Util\ExcelToJsonWizard.v1.0.6\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{787B72F0-8C2D-4CFA-B718-D065067EEF2E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80430D6C-F8C7-4F04-9E13-91569ADA2B50}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19245" windowHeight="8700" xr2:uid="{D930A799-48AB-4A51-887D-7090B3F85830}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>key</t>
   </si>
@@ -104,6 +104,14 @@
   </si>
   <si>
     <t>Shield</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Price</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이템 가격</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -516,7 +524,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -547,6 +555,9 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -564,6 +575,9 @@
       <c r="E2" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -581,6 +595,9 @@
       <c r="E3" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
@@ -598,6 +615,9 @@
       <c r="E4" s="6" t="s">
         <v>14</v>
       </c>
+      <c r="F4">
+        <v>60</v>
+      </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
@@ -617,6 +637,9 @@
       <c r="E5" s="6" t="s">
         <v>14</v>
       </c>
+      <c r="F5">
+        <v>70</v>
+      </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
     </row>
@@ -636,6 +659,9 @@
       <c r="E6" s="8" t="s">
         <v>14</v>
       </c>
+      <c r="F6">
+        <v>100</v>
+      </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
@@ -655,6 +681,9 @@
       <c r="E7" s="8" t="s">
         <v>18</v>
       </c>
+      <c r="F7">
+        <v>50</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
@@ -671,6 +700,9 @@
       </c>
       <c r="E8" s="8" t="s">
         <v>20</v>
+      </c>
+      <c r="F8">
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>